<commit_message>
New qeustions v20251103 version
</commit_message>
<xml_diff>
--- a/data/llm_cfs_report_questions.xlsx
+++ b/data/llm_cfs_report_questions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JackWu/git_project/llm_esc_report_analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JackWu/git_project/crc-streamlit-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5ED5AC-4C2B-ED4E-8EE0-DD81980A15D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B0F30F-0419-2942-9241-C742023CDA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1120" windowWidth="27640" windowHeight="15700" xr2:uid="{6CBA2F91-21DC-2F40-AEAC-6FED94901F29}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="204">
   <si>
     <t>id</t>
   </si>
@@ -35089,32 +35089,94 @@
     <t>Intestine, large, colon, status post right hemicolectomy, resection, adenocarcinoma, signet-ring cellIntestine, small, ileum, status post right hemicolectomy, resection, no evidence of malignancyLymph node, regional, lymphadenectomy, no evidence of metastasis (0/37)Intestine, small, proximal anastomosis, resection, no evidence of malignancyIntestine, large, distal anastomosis, resection, no evidence of malignancySoft tissue, peritoneal, resection, suture granulomaMACROSCOPIC1. Specimen Type subtotal colectomy (status post right hemicolectomy)2. Specimen Length   Small intestine 11 cm/  Large intestine 40 cm3. Tumor Site   Sigmoid4. Main tumor    *Tumor Configuration Infiltrative    *Tumor Size 3.3 x 2.0 cm; 1.5 x 1.0 cm   *Macroscopic Tumor Perforation Not identified    *Distance to the closest margin 3cm(distal margin)   *Depth of tumor invasion muscularis propria5. Non-tumorous part 2 Polyps(1) 4 cm away from anastomosis site, 2.5 x 1.5 x 0.5 cm(2) 9.5 cm away from distal margin, 0.7 x 0.4 x 0.3 cm6. Additional specimens"proximal" and "distal""peritoneal tumor" 5.2 x 3.5 x 2 cmRepresentative sections are taken and labeled as   A1,2 the larger polypA3,4 sigmoid tumor, the larger oneA5 sigmoid tumor, the smaller oneB1 "proximal"B2 "distal"C1 small intestineC2 anastomosis site of previous right hemicolectomyC3 non-tumor, and the smaller polypD1-3 regional lymph nodeE1,2 peritoneal tumorMICROSCOPIC1. Histologic TypeSignet-ring cell carcinoma (greater than 50% signet-ring cells) 2. Histologic Grade  High-grade (poorly differentiated to undifferentiated)3. Pathologic Staging (pTNM according to AJCC v.7)   (A) Primary Tumor (pT) pT2 Tumor invades muscularis propria   (B) Regional Lymph Nodes (pN) pN0 No regional lymph node metastasisNote Number examined 37; Number involved 0    (C) Distant Metastasis (pM)Not applicable  4. Histologic Features Suggestive of Microsatellite Instability    (A) Intratumoral Lymphocytic Response (tumor-infiltrating lymphocytes) None     (B) Peritumor Lymphocytic Response (Crohn-like response) None     (C) Tumor Subtype and DifferentiationHigh histologic grade (poorly differentiated)5. Margins    (A) Proximal Margin Uninvolved by invasive carcinoma   (B) Distal Margin Uninvolved by invasive carcinoma6. Lymphovascular Invasion absent7. Perineural Invasion absent8. Tumor Deposits (discontinuous extramural extension) absent9. Type of Polyp in Which Invasive Carcinoma Arose Indeterminate10. Treatment Effect Not applicable11. Additional Pathologic Findings    Tubular adenoma, two12. Comment(s)    The tumor shows signet-ring carcinoma cells arranged in sheets in the mucosa, or arranged in glandular structure floating in mucin pools. The carcinoma cells are positive for CK20, CDX2, negative for CK7, synaptophysin, chromogranin. The picture supports the diagnosis of signet ring cell carcinoma.   The specimen called "peritoneal tumor" shows a well-circumscribed lesion composed of mature adipose tissue with fibrosis and suture granuloma. Thick smooth muscle bundles, probably muscularis propria of certain visceral organ, are noted around the lesion.</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">7-10 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang TC"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>年</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3-5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang TC"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>年</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang TC"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>年</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="PingFang TC"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>年</t>
+    </r>
+  </si>
+  <si>
+    <t>發現惡性腫瘤，建議立即臨床評估與處置</t>
+  </si>
+  <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Sessile serrated adenoma, Transverse colon, 0.6 cm. (A)
-Tubular adenoma, Transverse colon, 0.4 cm. (B)
-Tubular adenoma, Descending colon, 0.3 cm. (C)
-Tubular adenoma, Sigmoid colon, 0.4 cm. (D)
+A: Hyperplastic polyp, Transverse colon, S/P EMR (Endoscopic mucosal resection), 0.6 x 0.4 x 0.3 cm.
+B: Tubular adenoma, Transverse colon, S/P EMR (Endoscopic mucosal resection), 0.3 x 0.3 x 0.3 cm.
+C:?, Descending colon, S/P EMR (Endoscopic mucosal resection), 0.2 x 0.2 x 0.2 cm.
+D: Tubular adenoma, Sigmoid colon, S/P EMR (Endoscopic mucosal resection), 0.8 x 0.5 x 0.4 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
-總腺瘤數: 3 (小於10mm: 3, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 1 (小於10mm: 1, 大於等於10mm: 0)
+總腺瘤數: 2 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
 高風險特徵:
   - 高度不典型增生: 否
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3-5 年</t>
+3. 2020_USMSTF 建議追蹤時間
+7-10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, A-colon, 0.3 cm. (A)
-Tubular adenoma, Hepatic flexure, 0.4 cm. (B)
-Tubular adenoma, Splenic flexure, 0.5 cm. (C)
-Hyperplastic polyp, S-colon, 0.8 cm.
+A: Tubular adenoma, Ascending colon, S/p biopsy, 0.1 x 0.1 x 0.1 cm.
+B: Tubular adenoma, Hepatic flexure, S/p biopsy, 0.1 x 0.1 x 0.1 cm.
+C: Tubular adenoma, Descending colon, S/p biopsy, 0.2 x 0.1 x 0.1 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35125,33 +35187,32 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 3-5 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Transverse colon, 4 cm. (A)
-Hyperplastic polyp, Transverse colon, 1 cm. (B)
-Tubular adenoma, Splenic flexure, 5 cm. (C)
-Tubular adenoma, Sigmoid colon, 2 cm. (D)
+A: Tubulovillous adenoma, Splenic flexure, S/p ESD, up to 3.2 x 2.0 x 0.5 cm.
+B: Hyperplastic polyp, Transverse colon, S/p biopsy, 1 cm.
+C: Tubular adenoma, Sigmoid colon, S/p biopsy, 2 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
-總腺瘤數: 3 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 3)
+總腺瘤數: 2 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 1)
 總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
 高風險特徵:
   - 高度不典型增生: 否
-  - 絨毛狀結構: 否
+  - 絨毛狀結構: 是
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 3 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Rectal nodular lesions with ulcer, 0.1-0.3 cm. (NIL), Rectum, NIL.
+A: Chronic proctitis, Rectum, S/p colonoscopic biopsy, up to 0.4 x 0.3 x 0.1 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35162,52 +35223,51 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubulovillous adenoma, Ascending colon, 1.8 cm. (A), Tubular adenoma, Sigmoid colon, 2 cm.
+A: Tubulovillous adenoma, Ascending colon, S/p EMR (Endoscopic mucosal resection), 1.7 x 1.2 x 0.6 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
-總腺瘤數: 2 (小於10mm: 0, 10-19mm: 1, 大於等於20mm: 1)
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
 總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
 高風險特徵:
   - 高度不典型增生: 否
   - 絨毛狀結構: 是
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 3 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, T-colon, 0.3 cm. (A)
-Tubular adenoma, S-colon, 0.3 cm. (B)
-Tubular adenoma, S-colon, 0.3 cm. (C)
-Tubular adenoma, Rectum, 0.2 cm. (D)
+A: Tubular adenoma, Transverse colon, S/p biopsy, 0.3 x 0.2 x 0.2 cm.
+B: Tubular adenoma, Sigmoid colon, S/p biopsy, 0.2 x 0.1 x 0.1 cm.
+C: Tubular adenoma, Sigmoid colon, S/p polypectomy, 0.2 x 0.1 x 0.1 cm.
+D: Tubular adenoma, Rectum, S/p biopsy, (no size mentioned).
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
-總腺瘤數: 4 (小於10mm: 4, 10-19mm: 0, 大於等於20mm: 0)
+總腺瘤數: 3 (小於10mm: 3, 10-19mm: 0, 大於等於20mm: 0)
 總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
 高風險特徵:
   - 高度不典型增生: 否
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 3-5 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Ascending colon, 0.3 cm. (A)
-Tubular adenoma, Ascending colon, 0.5 cm. (B)
-Mixed hemorrhoids
+A: Tubular adenoma, Ascending colon, S/p endoscopic mucosal resection and biopsy, 0.6 x 0.5 x 0.3 cm.
+B: Tubular adenoma, Ascending colon, S/p cold snare polypectomy, 0.5cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35218,14 +35278,14 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 7-10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Ascending colon, 0.6 cm. (A)
-Tubular adenoma, Ascending colon, 0.3 cm. (A)
+A: Tubular adenoma, Ascending colon, S/p biopsy and removal, 0.4 x 0.2 x 0.2 cm.
+B: Tubular adenoma, Ascending colon, S/p EMR (Endoscopic mucosal resection), S/p hemoclipping, 0.6 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35236,13 +35296,13 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 7-10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Transverse colon, 2 cm.
+A: Tubular adenoma, Transverse colon, S/p ESD (Endoscopic submucosal dissection), S/p hemoclipping, 2 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35253,53 +35313,53 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 3 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Ascending colon, 2.8 cm. (A)
-Tubular adenoma, Ascending colon, 1 cm. (B)
-Tubular adenoma, Hepatic flexure, 1 cm. (C)
-Tubular adenoma, Hepatic flexure, 0.8 cm. (D)
-Tubular adenoma, Transverse colon, 0.6 cm. (E)
-Tubular adenoma, Transverse colon, 0.4 cm. (F)
+A: Tubulovillous adenoma, Ascending colon, S/p ESD (Endoscopic submucosal dissection), 2.3 x 2.1 x 0.6 cm.
+B: Tubular adenoma, Ascending colon, S/p EMR (Endoscopic mucosal resection), 0.8 x 0.4 x 0.4 cm.
+C: Inflammatory polyp, Ascending colon, S/p EMR (Endoscopic mucosal resection), 0.3 x 0.1 x 0.1 cm.
+D: Tubular adenoma, Hepatic flexure, S/p EMR (Endoscopic mucosal resection), 1.1 x 0.4 x 0.2 cm.
+E: Tubular adenoma, Transverse colon, S/p EMR (Endoscopic mucosal resection), 0.3 x 0.3 x 0.3 cm.
+F: Tubular adenoma, Transverse colon, S/p EMR (Endoscopic mucosal resection), 0.3 x 0.3 x 0.1 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
-總腺瘤數: 6 (小於10mm: 3, 10-19mm: 2, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubulovillous adenoma, Rectum, 7 cm. (A)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 1)
+總腺瘤數: 5 (小於10mm: 5, 10-19mm: 0, 大於等於20mm: 0)
 總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
 高風險特徵:
   - 高度不典型增生: 否
   - 絨毛狀結構: 是
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 3 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Transverse colon, 0.2 cm. (A)
-Tubular adenoma, Sigmoid colon, 0.4 cm. (B)
+A: Tubulovillous adenoma, Rectum, S/p ESD (Endoscopic submucosal dissection), 6 x 4.3 x 0.5 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Transverse colon, S/p biopsy and removal, 0.3 x 0.3 x 0.2 cm.
+B: Tubular adenoma, Sigmoid colon, S/p EMR (Endoscopic mucosal resection), 1.6 x 0.7 x 0.3 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35310,13 +35370,13 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 7-10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Rectum, 0.4 cm. (A)
+A: Tubular adenoma, Rectum, S/p cold snare polypectomy, 0.4cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35327,13 +35387,13 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 7-10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Ascending colon, 0.6 cm. (A)
+A: Tubular adenoma, Rectum, S/p EMR (Endoscopic mucosal resection), 0.3 x 0.2 x 0.1 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35344,13 +35404,50 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 7-10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Traditional serrated adenoma, Rectum, 1.6 cm. (A)
+A: Tubular adenoma, Rectum, S/p EMR (Endoscopic mucosal resection), 0.9 x 0.6 x 0.5 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+7-10 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Cecum, S/p polypectomy, 0.3 x 0.3 x 0.2 cm.
+B: Tubular adenoma, Transverse colon, S/p polypectomy, 0.4 x 0.2 x 0.2 cm.
+C: Tubular adenoma, Transverse colon, S/p polypectomy, 0.3 x 0.7 x 0.1 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 3 (小於10mm: 3, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3-5 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Hyperplastic polyp, Ascending colon, S/p biopsy, 0.4 x 0.2 x 0.1 cm.
+B: Hyperplastic polyp, Ascending colon, S/p biopsy, 0.4 x 0.2 x 0.1 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35361,15 +35458,266 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
+10 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Cecum, S/p EMR (Endoscopic mucosal resection), 1.6 x 0.6 x 0.5 cm.
+B: Tubulovillous adenoma, Ascending colon, S/p ESD (Endoscopic submucosal dissection), 4.2 x 4.0 x 0.3 cm.
+C: Hyperplastic polyp, Transverse colon, S/p polypectomy, 0.4 x 0.3 x 0.2 cm.
+D: Tubular adenoma, Transverse colon, S/p EMR (Endoscopic mucosal resection), 0.8 x 0.6 x 0.4 cm.
+E: Tubular adenoma, Sigmoid colon, S/p EMR (Endoscopic mucosal resection), 1.2 x 0.8 x 0.5 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 4 (小於10mm: 4, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
 3 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Cecum, 0.4 cm. (A)
-Tubular adenoma, Transverse colon, 0.6 cm. (B)
-Tubular adenoma, Transverse colon, 0.3 cm. (C)
+A: Tubular adenoma, Transverse colon, S/p EMR (Endoscopic mucosal resection), 0.7cm.
+B: Tubular adenoma, Transverse colon, S/p EMR (Endoscopic mucosal resection), 0.5cm.
+C: Tubular adenoma, Transverse colon, S/p polypectomy, 0.6cm.
+D: Tubular adenoma, Transverse colon, S/p EMR (Endoscopic mucosal resection), 0.5cm.
+E: Tubulovillous adenoma, Transverse colon, S/p polypectomy, 0.7cm.
+F: Tubular adenoma, Transverse colon, S/p polypectomy, 0.3cm.
+G: ESD scar, Transverse colon, S/p biopsy, (no size mentioned).
+H: Tubulovillous adenoma, Transverse colon, S/p polypectomy, 1.2cm.
+I: Tubulovillous adenoma, Descending colon, S/p polypectomy, 1.2cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 8 (小於10mm: 6, 10-19mm: 2, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Transverse colon, S/p polypectomy, 1.2 x 0.5 x 0.2 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+7-10 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Transverse colon, S/p biopsy, 0.3 x 0.2 x 0.2 cm.
+B: Tubular adenoma, Transverse colon, S/p biopsy, 0.3 x 0.2 x 0.1 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 2 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+7-10 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Ascending colon, S/p EMR, 0.6 x 0.3 x 0.1 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+7-10 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubulovillous adenoma, Cecum, S/p EMR, 2.7 x 1.7 x 0.5 cm.
+Location: Cecum
+Procedure: Colonoscopic piecemeal mucosal resection
+Size: 2.7 x 1.7 x 0.5 cm
+B: Tubulovillous adenoma, Rectum, S/p ESD, 7.5 x 6.5 x 0.7 cm.
+Location: Rectum
+Procedure: Colonoscopic submucosal dissection
+Size: 7.5 x 6.5 x 0.7 cm
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 2 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Ascending colon, S/p hot biopsy and removal, 0.3 x 0.2 x 0.2 cm.
+B: Tubular adenoma, Transverse colon, S/p EMR, up to 0.6 x 0.4 x 0.3 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 2 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+7-10 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Rectum, S/p cold snare polypectomy, 1.0 x 0.4 x 0.3 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+7-10 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubulovillous adenoma, Cecum, S/p colonoscopic polypectomy, 0.7 x 0.4 x 0.4 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Sigmoid colon, S/p cold snare polypectomy, 0.8 x 0.6 x 0.6 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+7-10 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Ileocecal valve, S/p colonoscopic submucosal dissection, 1.5 x 1.4 x 0.3 cm.
+B: Tubulovillous adenoma, Transverse colon, S/p polypectomy, 0.2 x 0.2 x 0.2 cm.
+C: Tubulovillous adenoma, Transverse colon, S/p polypectomy, up to 0.4 x 0.3 x 0.1 cm.
+D: Tubular adenoma, Transverse colon, S/p polypectomy, up to 1.1 x 0.6 x 0.3 cm.
+E: Tubulovillous adenoma, Transverse colon, S/p polypectomy, 0.3 x 0.3 x 0.3 cm.
+F: Tubulovillous adenoma, Sigmoid colon, S/p polypectomy, 1.1 x 0.5 x 0.5 cm.
+G: Tubulovillous adenoma, Rectum, S/p EMR (Endoscopic mucosal resection), 0.8 x 0.8 x 0.5 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 7 (小於10mm: 7, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Sessile serrated adenoma, Cecum, S/p cold Snaring polypectomy, 1cm.
+Size: Not mentioned in the colonoscopic findings, but mentioned in the pathology report as 1cm.
+B: Tubular adenoma, Cecum, S/p ESD, 4.5 x 2.5 x 0.2 cm.
+Size: 4.5 x 2.5 x 0.2 cm (from pathology report)
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 1 (小於10mm: 0, 大於等於10mm: 1)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Sigmoid colon, S/p ESD (Endoscopic submucosal dissection), 1.7 x 1.4 x 0.3 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+7-10 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Ileocecal valve, S/p cold snare polypectomy, 0.6 x 0.3 x 0.3 cm.
+B: Tubular adenoma, Transverse colon, S/p ESD (Endoscopic submucosal dissection), 3.5 x 2.5 x 0.2 cm.
+C: Tubular adenoma, Sigmoid colon, S/p cold snare polypectomy, 1.5 x 0.5 x 0.2 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35380,13 +35728,146 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 3-5 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Colon adenoma, Cecum, 0.3 cm. (A), Colon adenoma, Cecum, 0.3 cm. (B)
+A: Tubular adenoma, Transverse colon, S/p cold Snaring polypectomy, 0.6 x 0.4 x 0.2 cm.
+B: Tubular adenoma, Descending colon, S/p cold Snaring polypectomy, 0.3 x 0.2 x 0.1 cm.
+C: Tubulovillous adenoma, Rectum, S/p cold Snaring polypectomy, 0.7 x 0.5 x 0.4 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 3 (小於10mm: 3, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubulovillous adenoma, Transverse colon, S/p biopsy, 0.3 x 0.2 x 0.1 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Granulation tissue, Sigmoid colon, S/p cold snare polypectomy, 0.3 x 0.2 x 0.1 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 0 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+10 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Ascending colon, S/p cold snare polypectomy, 0.4 x 0.3 x 0.3 cm.
+B: Tubular adenoma, Ascending colon, S/p cold snare polypectomy, 0.3 x 0.3 x 0.2 cm.
+C: Tubulovillous adenoma, Transverse colon, S/p ESD, 2.5 x 2.5 x 0.4 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 3 (小於10mm: 3, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Villous adenoma, Ascending colon, S/p ESD (Endoscopic submucosal dissection), 5.6 x 4.2 x 1.0 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 0, 10-19mm: 1, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Ascending colon, S/p cold snare polypectomy, 1.3 x 0.6 x 0.3 cm.
+B: Tubular adenoma, Ascending colon, S/p cold snare polypectomy, 0.6 x 0.5 x 0.3 cm.
+C: Tubular adenoma, Transverse colon, S/p cold snare polypectomy, 1.0 x 0.8 x 0.3 cm.
+D: Tubular adenoma, Ascending colon, S/p cold snare polypectomy, S/p hemoclipping, 1.0 x 0.7 x 0.5 cm.
+E: Tubular adenoma, Transverse colon, S/p cold snare polypectomy, S/p hemoclipping, 1.4 x 0.8 x 0.5 cm.
+F: Tubular adenoma, Sigmoid colon, S/p cold snare polypectomy, 0.8 x 0.7 x 0.3 cm.
+G: Mucosal tag, Sigmoid colon, S/p cold snare polypectomy, 1.4 x 0.7 x 0.1 cm.
+H: Tubular adenoma, Sigmoid colon, S/p cold snare polypectomy, 0.9 x 0.7 x 0.4 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 7 (小於10mm: 7, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Sigmoid colon, S/p cold snare polypectomy, 0.3 x 0.2 x 0.2 cm.
+B: Tubulovillous adenoma, Rectum, S/p ESD (Endoscopic submucosal dissection), 4.5 x 3.5 x 0.4 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 2 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Hyperplastic polyp, Sigmoid colon, S/p biopsy, Mucosectomy, 0.3 x 0.2 x 0.2 cm.
+B: Tubular adenoma, Ascending colon, S/p biopsy, Mucosectomy, 0.8 x 0.6 x 0.3 cm.
+C: Tubular adenoma, Transverse colon, S/p biopsy, 0.3 x 0.3 x 0.2 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35397,57 +35878,32 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 7-10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubulovillous adenoma, Cecum, 1 cm. (A)
-Tubular adenoma, Transverse colon, 0.5 cm. (C)
-Tubular adenoma, Transverse colon, 0.5 cm. (D)
-Tubulovillous adenoma, Sigmoid colon, 1 cm. (E)
+A: Tubular adenoma, Sigmoid colon, S/p biopsy, 0.4 x 0.3 x 0.1 cm.
+B: Tubular adenoma, A-colon, S/p biopsy and EMR, 4mm.
+C: Tubular adenoma, T-colon, S/p biopsy, 3-4mm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
-總腺瘤數: 4 (小於10mm: 2, 10-19mm: 2, 大於等於20mm: 0)
+總腺瘤數: 3 (小於10mm: 3, 10-19mm: 0, 大於等於20mm: 0)
 總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
 高風險特徵:
   - 高度不典型增生: 否
-  - 絨毛狀結構: 是
+  - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
+3. 2020_USMSTF 建議追蹤時間
+3-5 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Transverse colon, 0.7 cm. (A)
-Tubular adenoma, Transverse colon, 0.5 cm. (B)
-Tubular adenoma, Transverse colon, 0.6 cm. (C)
-Tubular adenoma, Transverse colon, 0.5 cm. (D)
-Tubulovillous adenoma, Transverse colon, 0.7 cm. (E)
-Tubular adenoma, Transverse colon, 0.3 cm. (F)
-Tubulovillous adenoma, Transverse colon, 1.2 cm. (H)
-Tubulovillous adenoma, Descending colon, 1.2 cm. (I)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 8 (小於10mm: 6, 10-19mm: 2, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Transverse colon, 0.3 cm. (A)
+A: Tubular adenoma, Transverse colon, S/p cold snare polypectomy, 0.4cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35458,33 +35914,97 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 7-10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Sessile serrated adenoma, Ascending colon, 0.6 cm. (A)
-Tubular adenoma, Hepatic flexure, 2.5 cm.
+A: Tubular adenoma, Ascending colon, S/p colonoscopic submucosal dissection, 2.3 x 1.5 x 0.1 cm.
+B: Tubular adenoma, Ascending colon, S/p cold snare polypectomy, 0.7 x 0.3 x 0.2 cm.
+C: Tubular adenoma, Transverse colon, S/p cold snare polypectomy, 0.4 x 0.3 x 0.2 cm.
+D: Tubular adenoma, Transverse colon, S/p cold snare polypectomy, 0.3 x 0.3 x 0.2 cm.
+E: Tubular adenoma, Transverse colon, S/p cold snare polypectomy, 0.4 x 0.2 x 0.2 cm.
+F: Tubular adenoma, Transverse colon, S/p cold snare polypectomy, 0.9 x 0.3 x 0.2 cm.
+G: Tubular adenoma, Transverse colon, S/p cold snare polypectomy, 0.3 x 0.3 x 0.2 cm.
+H: Tubular adenoma, Descending colon, S/p cold snare polypectomy, 0.8 x 0.3 x 0.2 cm.
+I: Tubular adenoma, Sigmoid colon, S/p cold snare polypectomy, 1.4 x 0.3 x 0.3 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 1)
+總腺瘤數: 9 (小於10mm: 9, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 否
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Ascending colon, S/p cold snare polypectomy, 0.5 x 0.3 x 0.2 cm.
+B: Tubular adenoma, Sigmoid colon, S/p cold snare polypectomy, 0.2 x 0.2 x 0.1 cm.
+C: Tubulovillous adenoma with focal adenocarcinoma, Sigmoid colon, S/p ESD, 3.3 x 3.0 x 0.4 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+發現惡性腫瘤，建議立即臨床評估與處置
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+發現惡性腫瘤，建議立即臨床評估與處置</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubulovillous adenoma, Descending colon, S/p hot snare polypectomy, 0.7 x 0.7 x 0.4 cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
+總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
+高風險特徵:
+  - 高度不典型增生: 否
+  - 絨毛狀結構: 是
+  - 分次切除: 否
+------------------------------------------------------------
+3. 2020_USMSTF 建議追蹤時間
+3 年</t>
+  </si>
+  <si>
+    <t>1. 原始報告:
+------------------------------------------------------------
+A: Tubular adenoma, Cecum, S/p cold snare polypectomy, 0.5cm.
+B: Hyperplastic polyp, Ascending colon, S/p cold snare polypectomy, 0.5cm.
+C: Tubular adenoma, Ascending colon, S/p cold snare polypectomy, 0.5cm.
+D: Hyperplastic polyp, Sigmoid colon, S/p cold snare polypectomy, 1cm.
+E: Hyperplastic polyp, Sigmoid colon, S/p cold snare polypectomy, 0.8cm.
+F: (No specific diagnosis or size mentioned)
+G: Sessile serrated adenoma, T-colon, S/p EMR, 0.6cm.
+H: Hyperplastic polyp, Rectum, S/p EMR, 0.8cm.
+------------------------------------------------------------
+2. 臨床發現摘要:
+------------------------------------------------------------
+總腺瘤數: 2 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 0)
 總無柄鋸齒狀息肉數: 1 (小於10mm: 1, 大於等於10mm: 0)
 高風險特徵:
   - 高度不典型增生: 否
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
+3. 2020_USMSTF 建議追蹤時間
+3-5 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Transverse colon, 0.5 cm. (A)
-Tubular adenoma, Transverse colon, 0.5 cm. (B)
-External hemorrhoids
+A: Tubular adenoma, Cecum, S/p colonoscopic polypectomy, 1.0 x 0.9 x 0.2 cm.
+B: Hyperplastic polyp, Ascending colon, S/p colonoscopic polypectomy, 0.5 x 0.4 x 0.1 cm.
+C: Tubular adenoma, Ascending colon, S/p colonoscopic polypectomy, 0.9 x 0.7 x 0.1 cm.
+D: Hyperplastic polyp, Sigmoid colon, S/p colonoscopic polypectomy, up to 1.0 x 0.6 x 0.1 cm.
+E: Hyperplastic polyp, Sigmoid colon, S/p colonoscopic polypectomy, up to 1.0 x 0.7 x 0.1 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35495,32 +36015,32 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 7-10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubulovillous adenoma, Cecum, 2.5 cm. (A)
-Tubulovillous adenoma, Rectum, 8 cm. (B)
+A: Tubular adenoma, Sigmoid colon, S/p cold snare polypectomy, 1.3 x 0.4 x 0.1 cm.
+B: Tubular adenoma, Rectum, S/p cold snare polypectomy, S/p APC (argon plasma coagulation), 0.3 x 0.3 x 0.1 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
-總腺瘤數: 2 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 2)
+總腺瘤數: 2 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 0)
 總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
 高風險特徵:
   - 高度不典型增生: 否
-  - 絨毛狀結構: 是
+  - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
+3. 2020_USMSTF 建議追蹤時間
+7-10 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, Ascending colon, 0.1 cm. (A)
-Tubular adenoma, Transverse colon, 2 cm. (B)
+A: Tubulovillous adenoma, Ascending colon, S/p ESD, 4cm.
+B: Tubular adenoma, Transverse colon, S/p cold snare polypectomy, 0.4cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35528,128 +36048,18 @@
 總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
 高風險特徵:
   - 高度不典型增生: 否
-  - 絨毛狀結構: 否
+  - 絨毛狀結構: 是
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 3 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubulovillous adenoma, Anus, 0.6 cm, APC (argon plasma coagulation)
-Tubular adenoma, Rectum, 0.4 cm, S/p cold snare polypectomy
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 2 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Cecum, 1.5 cm.
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 0, 10-19mm: 1, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Sigmoid colon, 0.5 cm. (A)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-7-10 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubulovillous adenoma, ICV, 2 cm. (A)
-Tubular adenoma, Transverse colon, 0.4 cm. (B)
-Tubulovillous adenoma, Transverse colon, 1.2 cm. (C)
-Tubulovillous adenoma, Transverse colon, 1.5 cm. (D)
-Tubular adenoma, Transverse colon, 0.5 cm. (E)
-Tubulovillous adenoma, Sigmoid colon, 1.5 cm. (F)
-Tubulovillous adenoma, Rectum, 1.5 cm. (G)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 7 (小於10mm: 2, 10-19mm: 4, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Sessile serrated adenoma, Cecum, 1 cm. (A)
-Tubulovillous adenoma, Transverse colon, 4.5 cm. (B)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 1 (小於10mm: 0, 大於等於10mm: 1)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubulovillous adenoma, Sigmoid colon, 2 cm. (A)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Transverse colon, 0.5 cm. (A)
-Tubular adenoma, Descending colon, 0.4 cm. (B)
-Tubular adenoma, Rectum, 0.6 cm. (C)
+A: Tubular adenoma, Cecum, S/p cold snare polypectomy, 0.5 x 0.2 x 0.1 cm.
+B: Tubular adenoma, Sigmoid colon, S/p cold snare polypectomy, up to 0.5 x 0.4 x 0.1 cm.
+C: Tubular adenoma, Sigmoid colon, S/p cold snare polypectomy, 0.7 x 0.4 x 0.2 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
@@ -35660,388 +36070,20 @@
   - 絨毛狀結構: 否
   - 分次切除: 否
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
+3. 2020_USMSTF 建議追蹤時間
 3-5 年</t>
   </si>
   <si>
     <t>1. 原始報告:
 ------------------------------------------------------------
-Tubular adenoma, ICV, 0.8 cm. (A)
-Tubular adenoma, Transverse colon, 4.0 cm. (B)
-Tubular adenoma, Sigmoid colon, 1.2 cm. (C)
+A: Signet-ring cell carcinoma, Sigmoid colon, S/p resection, 3.3 x 2.0 cm, 1.5 x 1.0 cm.
 ------------------------------------------------------------
 2. 臨床發現摘要:
 ------------------------------------------------------------
-總腺瘤數: 3 (小於10mm: 1, 10-19mm: 1, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
+發現惡性腫瘤，建議立即臨床評估與處置
 ------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubulovillous adenoma, Transverse colon, 2 cm. (A)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Villous adenoma, Sigmoid colon, 0.4 cm. (A)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Ascending colon, 0.8 cm. (A)
-Tubular adenoma, Ascending colon, 0.5 cm. (B)
-Tubulovillous adenoma, Transverse colon, 3.5 cm. (C)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 3 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Villous adenoma, Ascending colon, 6.5 cm. (A)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Ascending colon, 0.4 cm. (A)
-Tubular adenoma, Ascending colon, 0.8 cm. (B)
-Tubular adenoma, Transverse colon, 1.2 cm. (C)
-Tubular adenoma, Ascending colon, 1.3 cm. (D)
-Tubular adenoma, Transverse colon, 1.5 cm. (E)
-Tubular adenoma, Sigmoid colon, 1 cm. (F)
-Tubular adenoma, Sigmoid colon, 0.4 cm. (G)
-Tubular adenoma, Sigmoid colon, 1 cm. (H)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 8 (小於10mm: 3, 10-19mm: 5, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Sigmoid colon, 0.4 cm. (A)
-Tubulovillous adenoma, Rectum, 5.3 cm x 3.5 cm. (B)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 2 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, T colon, 0.6 cm.
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-7-10 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Colon polyp, Sigmoid colon, 2-5mm. (A)
-Tubular adenoma, Ascending colon, 4mm. (B)
-Villous adenoma, Ascending colon, 10mm. (B)
-Tubular adenoma, Transverse colon, 3mm. (C)
-Tubular adenoma, Transverse colon, 4mm. (C)
-Multiple hyperplastic polyps, Rectum, 1-2mm.
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 4 (小於10mm: 3, 10-19mm: 1, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Transverse colon, 0.4 cm. (A)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 1 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-7-10 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Ascending colon, 0.3 cm. (A)
-Tubular adenoma, Transverse colon, 0.4 cm. (B)
-Tubular adenoma, Transverse colon, 0.4 cm. (C)
-Tubular adenoma, Transverse colon, 0.7 cm. (D)
-Tubular adenoma, Transverse colon, 0.8 cm. (E)
-Tubular adenoma, Transverse colon, 0.5 cm. (F)
-Tubular adenoma, Transverse colon, 0.5 cm. (G)
-Tubular adenoma, Descending colon, 0.9 cm. (H)
-Tubular adenoma, Sigmoid colon, 0.5 cm. (I)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 9 (小於10mm: 9, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Ascending colon, 0.4 cm. (A)
-Tubular adenoma, Sigmoid colon, 1 cm. (B)
-Tubulovillous adenoma, Sigmoid colon, 3.5 cm. (C)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 3 (小於10mm: 1, 10-19mm: 1, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Lateral spreading tumor, Hepatic flexure, 4 cm. (A)
-Colon polyp, Descending colon, 0.5 cm. (B)
-Colon cancer, Sigmoid colon, NIL. (C)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 0 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-10 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Cecum, 0.5 cm. (A)
-Hyperplastic polyp, Ascending colon, 0.5 cm. (B)
-Tubular adenoma, Ascending colon, 0.5 cm. (C)
-Hyperplastic polyp, Sigmoid colon, 1 cm. (D)
-Hyperplastic polyp, Sigmoid colon, 0.8 cm. (E)
-Tubulovillous adenoma, ICV, 3 cm. (Not managed)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 3 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Hyperplastic polyp, Transverse colon, 0.5 cm. (A)
-Hyperplastic polyp, Transverse colon, 0.5 cm. (B)
-Hyperplastic polyp, Transverse colon, 0.6 cm. (C)
-Hyperplastic polyp, Transverse colon, 0.5 cm. (D)
-Hyperplastic polyp, Descending colon, 0.6 cm. (E)
-Hyperplastic polyp, Sigmoid colon, 0.7 cm. (F)
-Hyperplastic polyp, Sigmoid colon, 0.6 cm. (G)
-Hyperplastic polyp, Rectum, 0.6 cm. (H)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 0 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-10 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Sigmoid colon, 0.2 cm. (A)
-Tubular adenoma, Rectum, 0.5 cm. (B)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 2 (小於10mm: 2, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-7-10 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubulovillous adenoma, Ascending colon, 4 cm. (A)
-Tubular adenoma, Transverse colon, 0.4 cm. (B)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 2 (小於10mm: 1, 10-19mm: 0, 大於等於20mm: 1)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 是
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Tubular adenoma, Cecum, 0.3 cm. (A)
-Tubular adenoma, Sigmoid colon, 0.8 cm. (B)
-Tubular adenoma, Sigmoid colon, 1.0 cm. (C)
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 3 (小於10mm: 2, 10-19mm: 1, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-3 年</t>
-  </si>
-  <si>
-    <t>1. 原始報告:
-------------------------------------------------------------
-Negative finding, NIL, Anastomosis site, NIL.
-------------------------------------------------------------
-2. 臨床發現摘要:
-------------------------------------------------------------
-總腺瘤數: 0 (小於10mm: 0, 10-19mm: 0, 大於等於20mm: 0)
-總無柄鋸齒狀息肉數: 0 (小於10mm: 0, 大於等於10mm: 0)
-高風險特徵:
-  - 高度不典型增生: 否
-  - 絨毛狀結構: 否
-  - 分次切除: 否
-------------------------------------------------------------
-3. 2020_USMSTF_Recommendation
-10 年</t>
-  </si>
-  <si>
-    <t>10 年</t>
-  </si>
-  <si>
-    <t>3 年</t>
-  </si>
-  <si>
-    <t>3-5 年</t>
-  </si>
-  <si>
-    <t>7-10 年</t>
+3. 2020_USMSTF 建議追蹤時間
+發現惡性腫瘤，建議立即臨床評估與處置</t>
   </si>
 </sst>
 </file>
@@ -36085,7 +36127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -36093,51 +36135,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -36455,7 +36461,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E51"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36488,10 +36494,10 @@
         <v>99</v>
       </c>
       <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36505,10 +36511,10 @@
         <v>100</v>
       </c>
       <c r="D3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36522,10 +36528,10 @@
         <v>101</v>
       </c>
       <c r="D4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36539,10 +36545,10 @@
         <v>102</v>
       </c>
       <c r="D5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36556,10 +36562,10 @@
         <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>200</v>
+      <c r="E6" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36573,10 +36579,10 @@
         <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>201</v>
+      <c r="E7" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36590,10 +36596,10 @@
         <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>202</v>
+      <c r="E8" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36607,10 +36613,10 @@
         <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>202</v>
+      <c r="E9" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36624,10 +36630,10 @@
         <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>200</v>
+      <c r="E10" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36641,10 +36647,10 @@
         <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>200</v>
+      <c r="E11" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36658,10 +36664,10 @@
         <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>200</v>
+      <c r="E12" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36675,10 +36681,10 @@
         <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>202</v>
+      <c r="E13" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36692,10 +36698,10 @@
         <v>111</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>202</v>
+      <c r="E14" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36709,10 +36715,10 @@
         <v>112</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>202</v>
+      <c r="E15" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36726,10 +36732,10 @@
         <v>113</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>200</v>
+      <c r="E16" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36743,10 +36749,10 @@
         <v>114</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>201</v>
+      <c r="E17" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36760,10 +36766,10 @@
         <v>115</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>202</v>
+      <c r="E18" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36777,10 +36783,10 @@
         <v>116</v>
       </c>
       <c r="D19" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>200</v>
+      <c r="E19" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36794,10 +36800,10 @@
         <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>200</v>
+      <c r="E20" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36811,10 +36817,10 @@
         <v>118</v>
       </c>
       <c r="D21" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>202</v>
+      <c r="E21" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36828,10 +36834,10 @@
         <v>119</v>
       </c>
       <c r="D22" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>200</v>
+      <c r="E22" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36845,10 +36851,10 @@
         <v>120</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>202</v>
+      <c r="E23" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36862,10 +36868,10 @@
         <v>121</v>
       </c>
       <c r="D24" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>200</v>
+      <c r="E24" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36879,10 +36885,10 @@
         <v>122</v>
       </c>
       <c r="D25" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>200</v>
+      <c r="E25" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36896,10 +36902,10 @@
         <v>123</v>
       </c>
       <c r="D26" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>200</v>
+      <c r="E26" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36913,10 +36919,10 @@
         <v>124</v>
       </c>
       <c r="D27" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>200</v>
+      <c r="E27" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36930,10 +36936,10 @@
         <v>125</v>
       </c>
       <c r="D28" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>202</v>
+      <c r="E28" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36947,10 +36953,10 @@
         <v>126</v>
       </c>
       <c r="D29" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>200</v>
+      <c r="E29" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36964,10 +36970,10 @@
         <v>127</v>
       </c>
       <c r="D30" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>200</v>
+      <c r="E30" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36981,10 +36987,10 @@
         <v>128</v>
       </c>
       <c r="D31" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>200</v>
+      <c r="E31" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36998,10 +37004,10 @@
         <v>129</v>
       </c>
       <c r="D32" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>201</v>
+      <c r="E32" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37015,10 +37021,10 @@
         <v>130</v>
       </c>
       <c r="D33" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>200</v>
+      <c r="E33" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37032,10 +37038,10 @@
         <v>131</v>
       </c>
       <c r="D34" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>200</v>
+      <c r="E34" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37049,10 +37055,10 @@
         <v>132</v>
       </c>
       <c r="D35" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>200</v>
+      <c r="E35" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37066,10 +37072,10 @@
         <v>133</v>
       </c>
       <c r="D36" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>200</v>
+      <c r="E36" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37083,10 +37089,10 @@
         <v>134</v>
       </c>
       <c r="D37" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>200</v>
+      <c r="E37" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37100,10 +37106,10 @@
         <v>135</v>
       </c>
       <c r="D38" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>200</v>
+      <c r="E38" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37117,10 +37123,10 @@
         <v>136</v>
       </c>
       <c r="D39" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>200</v>
+      <c r="E39" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37134,10 +37140,10 @@
         <v>137</v>
       </c>
       <c r="D40" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>202</v>
+      <c r="E40" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37151,10 +37157,10 @@
         <v>138</v>
       </c>
       <c r="D41" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
-      <c r="E41" s="5" t="s">
-        <v>200</v>
+      <c r="E41" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37168,10 +37174,10 @@
         <v>139</v>
       </c>
       <c r="D42" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
-      <c r="E42" s="5" t="s">
-        <v>202</v>
+      <c r="E42" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37185,10 +37191,10 @@
         <v>140</v>
       </c>
       <c r="D43" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>200</v>
+      <c r="E43" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37202,10 +37208,10 @@
         <v>141</v>
       </c>
       <c r="D44" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>200</v>
+      <c r="E44" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37219,10 +37225,10 @@
         <v>142</v>
       </c>
       <c r="D45" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
-      <c r="E45" s="5" t="s">
-        <v>199</v>
+      <c r="E45" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37236,10 +37242,10 @@
         <v>143</v>
       </c>
       <c r="D46" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
-      <c r="E46" s="5" t="s">
-        <v>200</v>
+      <c r="E46" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37253,10 +37259,10 @@
         <v>144</v>
       </c>
       <c r="D47" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
-      <c r="E47" s="5" t="s">
-        <v>199</v>
+      <c r="E47" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37270,10 +37276,10 @@
         <v>145</v>
       </c>
       <c r="D48" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>202</v>
+      <c r="E48" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37287,10 +37293,10 @@
         <v>146</v>
       </c>
       <c r="D49" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
-      <c r="E49" s="5" t="s">
-        <v>200</v>
+      <c r="E49" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37304,10 +37310,10 @@
         <v>147</v>
       </c>
       <c r="D50" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
-      <c r="E50" s="5" t="s">
-        <v>200</v>
+      <c r="E50" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37321,10 +37327,10 @@
         <v>148</v>
       </c>
       <c r="D51" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>199</v>
+      <c r="E51" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified UI display and english version
</commit_message>
<xml_diff>
--- a/data/llm_cfs_report_questions.xlsx
+++ b/data/llm_cfs_report_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JackWu/git_project/crc-streamlit-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DFCD2E-0F1B-5D40-B04B-AFB8CE600E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617AC053-4267-A745-AC6D-D337E9DA751C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1120" windowWidth="27640" windowHeight="15700" xr2:uid="{6CBA2F91-21DC-2F40-AEAC-6FED94901F29}"/>
   </bookViews>
@@ -34826,147 +34826,6 @@
   </si>
   <si>
     <t>Intestine, large, colon, ascending, endoscopic mucosal resection and biopsy, tubular    adenoma, two  MACROSCOPIC DESCRIPTION    The specimen submitted consists of 2 tissue fragment measuring 0.6 x 0.5 x 0.3 cm in size fixed in formalin.   Grossly, they are yellow brown and soft.    All for section.Jar 0.MICROSCOPIC DESCRIPTION * Histological diagnosis Tubular adenoma of the colon, two  * High grade dysplasia (including severe dysplasia and carcinoma in situ) Absent * Invasive carcinoma Absent * Surgical margins Free</t>
-  </si>
-  <si>
-    <r>
-      <t>Soft tissue, inguinal, left, herniorrhaphy, hernia sac The specimen submitted consists of one tissue fragment measuring 3.5 x 3.5 x 0.5 cm in size in fresh state.Grossly, it is red and soft. Representative section is taken.   Jar 1Microscopically, it shows a hernia sac.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="PingFang TC"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>總院</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> S9816599[01]. Appendix, , appendectomy, acute suppurative appendicitis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="PingFang TC"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>總院</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> S1323543[01]. Intestine, large, colon, descending, endoscopic submucosal dissection, tubular adenoma with focal severe dysplasia</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="PingFang TC"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>總院</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> S1312472[01]. Stomach, greater curvature of upper body, endoscopic biopsy, hyperplastic polyp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="PingFang TC"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>總院</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> S1312467[01]. Intestine, large, colon, ascending, colonoscopic biopsy, tubular adenoma</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="PingFang TC"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>總院</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> S1008135[01]. Intestine, large, colon, left side, endoscopic biopsy, hyperplastic polyp[02]. Stomach, antrum and body, endoscopic biopsy, chronic gastritis, without Helicobacter infection</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="PingFang TC"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>總院</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> S0836225[01]. Stomach, antrum, endoscopic biopsy, chronic active gastritis, with Helicobacter infection</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="PingFang TC"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>總院</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> S0616969[01]. Stomach, antrum &amp; body, endoscopic biopsy, chronic gastritis, without Helicobacter infection</t>
-    </r>
-  </si>
-  <si>
-    <t>Prostate, right lateral, transrectal ultrasound-guided biopsy, benign prostate tissue Prostate, right medial, transrectal ultrasound-guided biopsy, benign prostate tissue Prostate, left medial, transrectal ultrasound-guided biopsy, benign prostate tissue Prostate, left lateral, transrectal ultrasound-guided biopsy, benign prostate tissue MACROSCOPYSites of biopsy A. Right lateral 7 cores (length up to 0.7 cm) B. Right medial 9 cores (length up to 0.9 cm) C. Left medial 6 cores (length up to 1.1 cm) D. Left lateral 3 cores (length up to 0.7 cm)All for sections and labeled asJar 0 A1. Right lateral B1. Right medial C1. Left medial D1. Left lateralMICROSCOPY1. Histological diagnosis A. Right lateral benign prostate tissue  B. Right medial benign prostate tissue  C. Left medial benign prostate tissue  D. Left lateral benign prostate tissue 2. Perineural invasion absent 3. Extraprostatic extension absent 4. Seminal vesicle invasion seminal vesicle not included 5. Comment Immunohistochemically, preserved basal cells can be seen in the P63 stain on sections B and C.</t>
   </si>
   <si>
     <t>Intestine, large, colon, ascending, colonoscopic submucosal dissection, tubulovillous adenomaIntestine, large, colon, ascending, bottle B, colonoscopic mucosal resection, tubular adenomaIntestine, large, colon, ascending, bottle C, colonoscopic mucosal resection, inflammatory polypIntestine, large, colon, hepatic flexure, colonoscopic mucosal resection, tubular adenomaIntestine, large, colon, transverse, bottle E, colonoscopic mucosal resection, tubular adenomaIntestine, large, colon, transverse, bottle F, colonoscopic mucosal resection, tubular adenomaMACROSCOPIC A   1 tissue fragment, 2.3  x 2.1 x 0.6 cm in size. B   1 tissue fragment, 0.8 x 0.4 x 0.4 cm in sizeC   1 tissue fragment, 0.3 x 0.1 x 0.1  cm in sizeD  1  tissue fragment, 1.1 x 0.4 x 0.2  cm in sizeE  1  tissue fragment, 0.3 x 0.3 x 0.3  cm in sizeF  1  tissue fragment, 0.3 x 0.3 x 0.1  cm in sizeAll for section and labeled asJar 0A bottle AB bottle BC bottle CD bottle DE bottle EF bottle FMICROSCOPIC * Histological diagnosis A Tubulovillous adenoma B Tubular adenoma C Inflammatory polyp D Tubular adenoma E Tubular adenoma F Tubular adenoma* High grade dysplasia (including severe dysplasia and carcinoma in situ) Absent* Invasive carcinoma Absent * Section margin Uninvolved in all sections* Comment(s) nil</t>
@@ -35060,9 +34919,6 @@
   </si>
   <si>
     <t>Intestine, large, colon, sigmoid, colonoscopic biopsy, hyperplastic polypIntestine, large, colon, ascending, colonoscopic biopsy and mucosectomy, tubular adenoma, twoIntestine, large, colon, transverse, colonoscopic biopsy, tubular adenoma The specimen is submitted in three separated bottles labeled as A sigmoid, B ascending ,and C transverse, respectively, fixed in formalin.The specimen labeled as A consists of 3 tissue fragments measuring up to 0.3 x 0.2 x 0.2 cm in size.  Grossly, they are yellowish white and soft.The specimen labeled as B consists of 2 tissue fragments measuring up to 0.8 x 0.6 x 0.3 cm in size.  Grossly, they are brown and soft.The specimen labeled as C consists of 3 tissue fragments measuring up to 0.3 x 0.3 x 0.2 cm in size.  Grossly, they are yellowish white and soft.  All for section and labeled asJar 0A sigmoid  B ascending  C transverseMicroscopically, the section A shows a hyperplastic polyp. The section B shows two tubular adenoma. The section C shows a tubular adenoma.</t>
-  </si>
-  <si>
-    <t>Stomach, antrum, anterior wall, endoscopic biopsy, chronic active gastritis, with Helicobacter infectionStomach, antrum, LC side, endoscopic biopsy, chronic active gastritis, with Helicobacter infectionStomach, middle body, LC side, endoscopic mucosal resection, inflammatory polyp    The specimens fixed in formalin are submitted in three parts, respectively labeled as A antrum, anterior wall, B antrum, LC side, and C middle body, LC side.    The specimen labeled as A consists of 2 tissue fragments measuring up to 0.5 x 0.3 x 0.2 cm in size. Grossly, they are yellowish and elastic.    The specimen labeled as B consists of 2 tissue fragments measuring up to 0.6 x 0.2 x 0.2 cm in size. Grossly, they are yellowish and elastic.    The specimen labeled as C consists of 1 tissue fragment measuring 1.4 x 1.2 x 0.8 cm in size. Grossly, it is yellowish and elastic.    All for sections and labeled as     Jar 0    A1 antrum, anterior wall    B1 antrum, LC side    C1 middle body, LC side    Microscopically, all sections show chronic active gastritis with foci ofneutrophil and lymphoplasma cells infiltration in the mucosal glands and lamina propria. Focal incomplete intestinal metaplasia and formation of lymphoid follicle are also noted. Erosion was focally seen and atypical change of few glands are also noted in sections B and C. Many rod-like Helicobacter bacilli in the foveolar pits are demonstrated in all sections. CDX2- and CK-immunostain performed on section C shows no presence of atypical cells in inflamed lamina propria.</t>
   </si>
   <si>
     <t>Intestine,large,colon,ascending,proximal,A,colonoscopic submucosal dissection, tubular adenomaIntestine,large,colon,ascending,B,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,C,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,D,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,E,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,F,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,G,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,descending,H,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,sigmoid,I,colonoscopic cold snare polypectomy, tubular adenomaMACROSCOPIC A One tissue fragment, 2.3 x 1.5 x 0.1 cm in sizeB One tissue fragment, 0.7 x 0.3 x 0.2 cm in sizeC One tissue fragment, 0.4 x 0.3 x 0.2 cm in sizeD One tissue fragment, 0.3 x 0.3 x 0.2 cm in sizeE Three tissue fragments, up to 0.4 x 0.2 x 0.2 cm in sizeF One tissue fragment, 0.9 x 0.3 x 0.2 cm in sizeG One tissue fragment, 0.3 x 0.3 x 0.2 cm in sizeH Three tissue fragments, up to 0.8 x 0.3 x 0.2 cm in sizeI One tissue fragment, 1.4 x 0.3 x 0.3 cm in sizeAll for sections and labeled asJar 0A1,B1 A-colonC1-G1 T-colonH1 D-colonI1 S-colonMICROSCOPIC * Histological diagnosis A1 Tubular adenoma B1 Tubular adenoma C1 Tubular adenoma D1 Tubular adenoma E1 Tubular adenoma F1 Tubular adenoma G1 Tubular adenoma H1 Tubular adenoma I1 Tubular adenoma* High grade dysplasia (including severe dysplasia and carcinoma in situ) Absent * Invasive carcinoma Absent  * Surgical margin     Section A1Uninvolved(Horizontal2 mm,Vertical 1.5 mm)Section B1-I1 Uninvolved     * Commentnil</t>
@@ -36037,6 +35893,15 @@
   <si>
     <t>Malignancy found, immediate clinical evaluation and management recommended</t>
   </si>
+  <si>
+    <t>Intestine, large, colon, transverse, endoscopic submucosal dissection, tubular adenomaMACROSCOPIC *Quantity 4 tissue fragments, up to 1.5 x 0.8 x 0.5 cm in sizeAll for section Jar 0MICROSCOPIC * Histological diagnosis    Tubular adenoma* High grade dysplasia (including severe dysplasia and carcinoma in situ)    Absent* Invasive carcinoma Absent * Surgical margin    Uninvolved * Comment(s) Dysplastic cells form tubular glands with hyperchromasia and elongated nuclei. It is compatible with tubular adenoma.Refnil</t>
+  </si>
+  <si>
+    <t>Intestine, large, colon, ascending, colonoscopic submucosal dissection, tubulovillous adenomaIntestine, large, colon, ascending, bottle B, colonoscopic mucosal resection, tubular adenomaIntestine, large, colon, ascending, bottle C, colonoscopic mucosal resection, inflammatory polypIntestine, large, colon, hepatic flexure, colonoscopic mucosal resection, tubular adenomaIntestine, large, colon, transverse, bottle E, colonoscopic mucosal resection, tubular adenomaIntestine, large, colon, transverse, bottle F, colonoscopic mucosal resection, tubular adenomaMACROSCOPIC A   1 tissue fragment, 2.3  x 2.1 x 0.6 cm in size. B   1 tissue fragment, 0.8 x 0.4 x 0.4 cm in sizeC   1 tissue fragment, 0.3 x 0.1 x 0.1  cm in sizeD  1  tissue fragment, 1.1 x 0.4 x 0.2  cm in sizeE  1  tissue fragment, 0.3 x 0.3 x 0.3  cm in sizeF  1  tissue fragment, 0.3 x 0.3 x 0.1  cm in sizeAll for section and labeled asJar 0A bottle AB bottle BC bottle CD bottle DE bottle EF bottle FMICROSCOPIC * Histological diagnosis A Tubulovillous adenoma B Tubular adenoma C Inflammatory polyp D Tubular adenoma E Tubular adenoma F Tubular adenoma* High grade dysplasia (including severe dysplasia and carcinoma in situ) Absent* Invasive carcinoma Absent * Section margin Uninvolved in all sections* Comment(s) nilRef Nil</t>
+  </si>
+  <si>
+    <t>Intestine,large,colon,ascending,proximal,A,colonoscopic submucosal dissection, tubular adenomaIntestine,large,colon,ascending,B,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,C,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,D,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,E,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,F,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,G,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,descending,H,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,sigmoid,I,colonoscopic cold snare polypectomy, tubular adenomaMACROSCOPIC A One tissue fragment, 2.3 x 1.5 x 0.1 cm in sizeB One tissue fragment, 0.7 x 0.3 x 0.2 cm in sizeC One tissue fragment, 0.4 x 0.3 x 0.2 cm in sizeD One tissue fragment, 0.3 x 0.3 x 0.2 cm in sizeE Three tissue fragments, up to 0.4 x 0.2 x 0.2 cm in sizeF One tissue fragment, 0.9 x 0.3 x 0.2 cm in sizeG One tissue fragment, 0.3 x 0.3 x 0.2 cm in sizeH Three tissue fragments, up to 0.8 x 0.3 x 0.2 cm in sizeI One tissue fragment, 1.4 x 0.3 x 0.3 cm in sizeAll for sections and labeled asJar 0A1,B1 A-colonC1-G1 T-colonH1 D-colonI1 S-colonMICROSCOPIC * Histological diagnosis A1 Tubular adenoma B1 Tubular adenoma C1 Tubular adenoma D1 Tubular adenoma E1 Tubular adenoma F1 Tubular adenoma G1 Tubular adenoma H1 Tubular adenoma I1 Tubular adenoma* High grade dysplasia (including severe dysplasia and carcinoma in situ) Absent * Invasive carcinoma Absent  * Surgical margin     Section A1Uninvolved(Horizontal2 mm,Vertical 1.5 mm)Section B1-I1 Uninvolved     * CommentnilRefNilRefnil.</t>
+  </si>
 </sst>
 </file>
 
@@ -36412,8 +36277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49916D18-5A43-4849-AEA9-6BB3DABC5BE3}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36446,10 +36311,10 @@
         <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36463,10 +36328,10 @@
         <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36480,10 +36345,10 @@
         <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36497,10 +36362,10 @@
         <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36514,10 +36379,10 @@
         <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36531,10 +36396,10 @@
         <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36548,10 +36413,10 @@
         <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36565,10 +36430,10 @@
         <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36579,13 +36444,13 @@
         <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>107</v>
+        <v>201</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36596,13 +36461,13 @@
         <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="D11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36613,13 +36478,13 @@
         <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D12" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36630,13 +36495,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36647,13 +36512,13 @@
         <v>29</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36664,13 +36529,13 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36681,13 +36546,13 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36698,13 +36563,13 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36715,13 +36580,13 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36732,13 +36597,13 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36749,13 +36614,13 @@
         <v>40</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D20" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36766,13 +36631,13 @@
         <v>42</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36783,13 +36648,13 @@
         <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36800,13 +36665,13 @@
         <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36817,13 +36682,13 @@
         <v>47</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36834,13 +36699,13 @@
         <v>49</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D25" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36851,13 +36716,13 @@
         <v>51</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D26" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36868,13 +36733,13 @@
         <v>53</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D27" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36885,13 +36750,13 @@
         <v>55</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36902,13 +36767,13 @@
         <v>57</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D29" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36919,13 +36784,13 @@
         <v>59</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D30" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36936,13 +36801,13 @@
         <v>61</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36953,13 +36818,13 @@
         <v>63</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D32" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36970,13 +36835,13 @@
         <v>64</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D33" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36987,13 +36852,13 @@
         <v>66</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D34" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37004,13 +36869,13 @@
         <v>68</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D35" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37021,13 +36886,13 @@
         <v>70</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D36" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37038,13 +36903,13 @@
         <v>72</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D37" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37055,13 +36920,13 @@
         <v>74</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D38" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37072,13 +36937,13 @@
         <v>76</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D39" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37089,13 +36954,13 @@
         <v>78</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37106,13 +36971,13 @@
         <v>79</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D41" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37123,13 +36988,13 @@
         <v>81</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D42" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37140,13 +37005,13 @@
         <v>83</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>140</v>
+        <v>203</v>
       </c>
       <c r="D43" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37157,13 +37022,13 @@
         <v>85</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D44" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37174,13 +37039,13 @@
         <v>87</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D45" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37191,13 +37056,13 @@
         <v>89</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D46" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37208,13 +37073,13 @@
         <v>90</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D47" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37225,13 +37090,13 @@
         <v>92</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D48" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37242,13 +37107,13 @@
         <v>94</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D49" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37259,13 +37124,13 @@
         <v>96</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D50" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37276,16 +37141,17 @@
         <v>98</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D51" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified accuracy measure  version
</commit_message>
<xml_diff>
--- a/data/llm_cfs_report_questions.xlsx
+++ b/data/llm_cfs_report_questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JackWu/git_project/crc-streamlit-app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617AC053-4267-A745-AC6D-D337E9DA751C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88D478C-ED23-EF45-95D5-6AB857C3396C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1120" windowWidth="27640" windowHeight="15700" xr2:uid="{6CBA2F91-21DC-2F40-AEAC-6FED94901F29}"/>
+    <workbookView xWindow="34460" yWindow="1900" windowWidth="27640" windowHeight="15700" xr2:uid="{6CBA2F91-21DC-2F40-AEAC-6FED94901F29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35879,21 +35879,6 @@
 Malignancy found, immediate clinical evaluation and management recommended</t>
   </si>
   <si>
-    <t>7-10 Years</t>
-  </si>
-  <si>
-    <t>3-5 Years</t>
-  </si>
-  <si>
-    <t>3 Years</t>
-  </si>
-  <si>
-    <t>10 Years</t>
-  </si>
-  <si>
-    <t>Malignancy found, immediate clinical evaluation and management recommended</t>
-  </si>
-  <si>
     <t>Intestine, large, colon, transverse, endoscopic submucosal dissection, tubular adenomaMACROSCOPIC *Quantity 4 tissue fragments, up to 1.5 x 0.8 x 0.5 cm in sizeAll for section Jar 0MICROSCOPIC * Histological diagnosis    Tubular adenoma* High grade dysplasia (including severe dysplasia and carcinoma in situ)    Absent* Invasive carcinoma Absent * Surgical margin    Uninvolved * Comment(s) Dysplastic cells form tubular glands with hyperchromasia and elongated nuclei. It is compatible with tubular adenoma.Refnil</t>
   </si>
   <si>
@@ -35901,6 +35886,21 @@
   </si>
   <si>
     <t>Intestine,large,colon,ascending,proximal,A,colonoscopic submucosal dissection, tubular adenomaIntestine,large,colon,ascending,B,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,C,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,D,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,E,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,F,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,transverse,G,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,descending,H,colonoscopic cold snare polypectomy, tubular adenomaIntestine,large,colon,sigmoid,I,colonoscopic cold snare polypectomy, tubular adenomaMACROSCOPIC A One tissue fragment, 2.3 x 1.5 x 0.1 cm in sizeB One tissue fragment, 0.7 x 0.3 x 0.2 cm in sizeC One tissue fragment, 0.4 x 0.3 x 0.2 cm in sizeD One tissue fragment, 0.3 x 0.3 x 0.2 cm in sizeE Three tissue fragments, up to 0.4 x 0.2 x 0.2 cm in sizeF One tissue fragment, 0.9 x 0.3 x 0.2 cm in sizeG One tissue fragment, 0.3 x 0.3 x 0.2 cm in sizeH Three tissue fragments, up to 0.8 x 0.3 x 0.2 cm in sizeI One tissue fragment, 1.4 x 0.3 x 0.3 cm in sizeAll for sections and labeled asJar 0A1,B1 A-colonC1-G1 T-colonH1 D-colonI1 S-colonMICROSCOPIC * Histological diagnosis A1 Tubular adenoma B1 Tubular adenoma C1 Tubular adenoma D1 Tubular adenoma E1 Tubular adenoma F1 Tubular adenoma G1 Tubular adenoma H1 Tubular adenoma I1 Tubular adenoma* High grade dysplasia (including severe dysplasia and carcinoma in situ) Absent * Invasive carcinoma Absent  * Surgical margin     Section A1Uninvolved(Horizontal2 mm,Vertical 1.5 mm)Section B1-I1 Uninvolved     * CommentnilRefNilRefnil.</t>
+  </si>
+  <si>
+    <t>7-10y</t>
+  </si>
+  <si>
+    <t>3y</t>
+  </si>
+  <si>
+    <t>3-5y</t>
+  </si>
+  <si>
+    <t>10y</t>
+  </si>
+  <si>
+    <t>malignancy</t>
   </si>
 </sst>
 </file>
@@ -36277,8 +36277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49916D18-5A43-4849-AEA9-6BB3DABC5BE3}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="171" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36314,7 +36314,7 @@
         <v>146</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36331,7 +36331,7 @@
         <v>147</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36348,7 +36348,7 @@
         <v>148</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36365,7 +36365,7 @@
         <v>149</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36382,7 +36382,7 @@
         <v>150</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36399,7 +36399,7 @@
         <v>151</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36416,7 +36416,7 @@
         <v>152</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36433,7 +36433,7 @@
         <v>153</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36444,13 +36444,13 @@
         <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D10" t="s">
         <v>154</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36461,13 +36461,13 @@
         <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D11" t="s">
         <v>155</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36484,7 +36484,7 @@
         <v>156</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36501,7 +36501,7 @@
         <v>157</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36518,7 +36518,7 @@
         <v>158</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36535,7 +36535,7 @@
         <v>159</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36552,7 +36552,7 @@
         <v>160</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36569,7 +36569,7 @@
         <v>161</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36586,7 +36586,7 @@
         <v>162</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36603,7 +36603,7 @@
         <v>163</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36620,7 +36620,7 @@
         <v>164</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36637,7 +36637,7 @@
         <v>165</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36654,7 +36654,7 @@
         <v>166</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36671,7 +36671,7 @@
         <v>167</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36688,7 +36688,7 @@
         <v>168</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36705,7 +36705,7 @@
         <v>169</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36722,7 +36722,7 @@
         <v>170</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36739,7 +36739,7 @@
         <v>171</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36756,7 +36756,7 @@
         <v>172</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36773,7 +36773,7 @@
         <v>173</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36790,7 +36790,7 @@
         <v>174</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36807,7 +36807,7 @@
         <v>175</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36824,7 +36824,7 @@
         <v>176</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36841,7 +36841,7 @@
         <v>177</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36858,7 +36858,7 @@
         <v>178</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36875,7 +36875,7 @@
         <v>179</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36892,7 +36892,7 @@
         <v>180</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36909,7 +36909,7 @@
         <v>181</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36926,7 +36926,7 @@
         <v>182</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36943,7 +36943,7 @@
         <v>183</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36960,7 +36960,7 @@
         <v>184</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36977,7 +36977,7 @@
         <v>185</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -36994,7 +36994,7 @@
         <v>186</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37005,13 +37005,13 @@
         <v>83</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D43" t="s">
         <v>187</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37028,7 +37028,7 @@
         <v>188</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37045,7 +37045,7 @@
         <v>189</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37062,7 +37062,7 @@
         <v>190</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37079,7 +37079,7 @@
         <v>191</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37096,7 +37096,7 @@
         <v>192</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37113,7 +37113,7 @@
         <v>193</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37130,7 +37130,7 @@
         <v>194</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.25">
@@ -37147,7 +37147,7 @@
         <v>195</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>